<commit_message>
Working Android version. System for loading audio and scenarios changed so that it could be loaded from Resources. Account panel for SUGAR added so that this step can be passed during testing on Android.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Localization/SUGAR Unity Localization.xlsx
+++ b/Assets/Resources/Localization/SUGAR Unity Localization.xlsx
@@ -199,9 +199,6 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>Password:</t>
-  </si>
-  <si>
     <t>POSITION</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>USERNAME</t>
   </si>
   <si>
-    <t>Username:</t>
-  </si>
-  <si>
     <t>VALUE</t>
   </si>
   <si>
@@ -266,6 +260,12 @@
   </si>
   <si>
     <t>nl</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -615,10 +615,10 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -950,8 +950,8 @@
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>61</v>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>4</v>
@@ -959,10 +959,10 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
@@ -970,10 +970,10 @@
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>41</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>4</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>4</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>4</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>4</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>4</v>
@@ -1072,7 +1072,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>4</v>

</xml_diff>